<commit_message>
downloaded satinsky 2015 metadata for bac ab and chl macapa may 11
</commit_message>
<xml_diff>
--- a/analyses/T7-incubations/unipept/GO/primary-prod/stations-grouped.xlsx
+++ b/analyses/T7-incubations/unipept/GO/primary-prod/stations-grouped.xlsx
@@ -203,8 +203,8 @@
   </sheetPr>
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N57" activeCellId="0" sqref="N57"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G29" activeCellId="0" sqref="G29:M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -709,6 +709,9 @@
       <c r="E24" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="G24" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="L24" s="0" t="n">
         <v>1</v>
       </c>
@@ -758,6 +761,12 @@
       <c r="E26" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="L26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M26" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
@@ -785,7 +794,7 @@
       </c>
       <c r="G28" s="0" t="n">
         <f aca="false">SUM(G24:G27)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H28" s="0" t="n">
         <f aca="false">SUM(H24:H27)</f>
@@ -805,15 +814,15 @@
       </c>
       <c r="L28" s="0" t="n">
         <f aca="false">SUM(L24:L27)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M28" s="0" t="n">
         <f aca="false">SUM(M24:M27)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N28" s="0" t="n">
         <f aca="false">SUM(G28:M28)</f>
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -822,7 +831,7 @@
       </c>
       <c r="G29" s="0" t="n">
         <f aca="false">G28/$N$28</f>
-        <v>0.166666666666667</v>
+        <v>0.363636363636364</v>
       </c>
       <c r="H29" s="0" t="n">
         <f aca="false">H28/$N$28</f>
@@ -830,23 +839,23 @@
       </c>
       <c r="I29" s="0" t="n">
         <f aca="false">I28/$N$28</f>
-        <v>0.166666666666667</v>
+        <v>0.0909090909090909</v>
       </c>
       <c r="J29" s="0" t="n">
         <f aca="false">J28/$N$28</f>
-        <v>0.166666666666667</v>
+        <v>0.0909090909090909</v>
       </c>
       <c r="K29" s="0" t="n">
         <f aca="false">K28/$N$28</f>
-        <v>0.166666666666667</v>
+        <v>0.0909090909090909</v>
       </c>
       <c r="L29" s="0" t="n">
         <f aca="false">L28/$N$28</f>
-        <v>0.166666666666667</v>
+        <v>0.181818181818182</v>
       </c>
       <c r="M29" s="0" t="n">
         <f aca="false">M28/$N$28</f>
-        <v>0.166666666666667</v>
+        <v>0.181818181818182</v>
       </c>
       <c r="N29" s="0" t="n">
         <f aca="false">N28/$N$28</f>

</xml_diff>